<commit_message>
Customise.py is now more flexible with parameters and Froala forms
</commit_message>
<xml_diff>
--- a/media/excel-reader-test.xlsx
+++ b/media/excel-reader-test.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rajn/PycharmProjects/TaaraMail/mail_sender/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rajn/PycharmProjects/TaaraMail/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{788FBBB2-5937-7F4B-9C40-45D7076B32CB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8D33D52-5AE9-9049-9424-6627360AA2C5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3180" yWindow="2060" windowWidth="27640" windowHeight="16940" xr2:uid="{BB956867-4E80-2549-9E3C-F98421C8FBD8}"/>
   </bookViews>
@@ -550,7 +550,7 @@
   <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>